<commit_message>
Performance targets added to increment_chipspecs. Top students from 2016
I'm coming for you guys...
</commit_message>
<xml_diff>
--- a/documents/increment_chipspecs.xlsx
+++ b/documents/increment_chipspecs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02 Github\sha1_hash_upgrade\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{668C89C3-BC16-4194-BBE1-37226E3FEC7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37422B49-9020-4741-9DBF-4B12C11D01FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21120" yWindow="8130" windowWidth="38700" windowHeight="15435" xr2:uid="{17DD5A21-F35B-447A-9399-CCDA76C95FF3}"/>
+    <workbookView xWindow="0" yWindow="5565" windowWidth="38700" windowHeight="15435" xr2:uid="{17DD5A21-F35B-447A-9399-CCDA76C95FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ALUTS</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Area x delay</t>
   </si>
   <si>
-    <t>Increment 0 (starting point)</t>
-  </si>
-  <si>
     <t>FMAX (slow 900mv 100C) MHz</t>
   </si>
   <si>
@@ -52,6 +49,30 @@
   </si>
   <si>
     <t>Delay (ns)</t>
+  </si>
+  <si>
+    <t>Performance Targets (Top Students from 2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARGET #1 (Delay) [Samuel Bauza &amp; Michael Petrucci] </t>
+  </si>
+  <si>
+    <t>TARGET #2 (Delay) [Jinzhe Zhang]</t>
+  </si>
+  <si>
+    <t>TARGET #3 (Delay) [Kevin Pan &amp; Brandon Ustaris]</t>
+  </si>
+  <si>
+    <t>TARGET #1 (Area x Delay) [Jinzhe Zhang]</t>
+  </si>
+  <si>
+    <t>TARGET #2 (Area x Delay) [Kevin Pan &amp; Brandon Ustaris]</t>
+  </si>
+  <si>
+    <t>TARGET #3 (Area x Delay) [Rui Han]</t>
+  </si>
+  <si>
+    <t>Increment 0 (starting point) [Winter 2016]</t>
   </si>
 </sst>
 </file>
@@ -67,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,8 +107,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -95,11 +122,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -108,6 +164,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,15 +484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66856F66-09A0-410F-AAD3-522B3B10449F}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
@@ -452,16 +514,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -469,7 +531,7 @@
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>1842</v>
@@ -499,6 +561,318 @@
         <f>D2*H2*(10^-9)</f>
         <v>5.7423924093527624E-3</v>
       </c>
+    </row>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1319</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1508</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" ref="D3:D39" si="0">B26+C26</f>
+        <v>2827</v>
+      </c>
+      <c r="E26" s="4">
+        <v>186.15</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" ref="F3:F39" si="1">(1/E26)*1000</f>
+        <v>5.3720118184260004</v>
+      </c>
+      <c r="G26" s="4">
+        <v>146</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" ref="H3:H39" si="2">F26*G26</f>
+        <v>784.31372549019602</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" ref="I3:I39" si="3">D26*H26*(10^-9)</f>
+        <v>2.2172549019607844E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4">
+        <v>594</v>
+      </c>
+      <c r="C27" s="4">
+        <v>968</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="0"/>
+        <v>1562</v>
+      </c>
+      <c r="E27" s="4">
+        <v>321.23</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="1"/>
+        <v>3.1130342745073625</v>
+      </c>
+      <c r="G27" s="4">
+        <v>252</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="2"/>
+        <v>784.48463717585537</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="3"/>
+        <v>1.2253650032686863E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="4">
+        <v>559</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1007</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>1566</v>
+      </c>
+      <c r="E28" s="4">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="1"/>
+        <v>3.0759766225776679</v>
+      </c>
+      <c r="G28" s="4">
+        <v>258</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="2"/>
+        <v>793.60196862503835</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="3"/>
+        <v>1.2427806828668102E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="4">
+        <v>594</v>
+      </c>
+      <c r="C30" s="4">
+        <v>968</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="0"/>
+        <v>1562</v>
+      </c>
+      <c r="E30" s="4">
+        <v>321.23</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="1"/>
+        <v>3.1130342745073625</v>
+      </c>
+      <c r="G30" s="4">
+        <v>252</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="2"/>
+        <v>784.48463717585537</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="3"/>
+        <v>1.2253650032686863E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="4">
+        <v>559</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1007</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="0"/>
+        <v>1566</v>
+      </c>
+      <c r="E31" s="4">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="1"/>
+        <v>3.0759766225776679</v>
+      </c>
+      <c r="G31" s="4">
+        <v>258</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="2"/>
+        <v>793.60196862503835</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="3"/>
+        <v>1.2427806828668102E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="4">
+        <v>786</v>
+      </c>
+      <c r="C32" s="4">
+        <v>897</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="0"/>
+        <v>1683</v>
+      </c>
+      <c r="E32" s="4">
+        <v>293.17</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="1"/>
+        <v>3.4109902104580958</v>
+      </c>
+      <c r="G32" s="4">
+        <v>249</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="2"/>
+        <v>849.33656240406583</v>
+      </c>
+      <c r="I32" s="5">
+        <f t="shared" si="3"/>
+        <v>1.4294334345260429E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="9:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>